<commit_message>
Correct paths for referencing templates and/or paths within custom prompt fields.
</commit_message>
<xml_diff>
--- a/app/config/tables/agriculture/forms/agriculture/agriculture.xlsx
+++ b/app/config/tables/agriculture/forms/agriculture/agriculture.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\toolsuite\app-designer\app\config\tables\agriculture\forms\agriculture\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="1480" windowWidth="35040" windowHeight="20420" tabRatio="500"/>
+    <workbookView xWindow="3535" yWindow="1479" windowWidth="35044" windowHeight="20422" tabRatio="500" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -569,6 +574,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -898,30 +906,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" style="5" customWidth="1"/>
-    <col min="2" max="2" width="21.5" style="5" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" style="5" customWidth="1"/>
     <col min="3" max="3" width="29.6640625" style="5" customWidth="1"/>
     <col min="4" max="4" width="21" style="5" customWidth="1"/>
     <col min="5" max="5" width="16" style="5" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="36.5" style="5" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="36.44140625" style="5" customWidth="1"/>
     <col min="8" max="8" width="13.6640625" style="5" customWidth="1"/>
     <col min="9" max="9" width="20" style="5" customWidth="1"/>
-    <col min="10" max="10" width="30.5" style="5" customWidth="1"/>
+    <col min="10" max="10" width="30.44140625" style="5" customWidth="1"/>
     <col min="11" max="12" width="43" style="5" customWidth="1"/>
-    <col min="13" max="13" width="11.1640625" style="6" customWidth="1"/>
-    <col min="14" max="14" width="31.5" style="5" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" style="6" customWidth="1"/>
+    <col min="14" max="14" width="31.44140625" style="5" customWidth="1"/>
     <col min="15" max="15" width="26.6640625" style="5" customWidth="1"/>
-    <col min="16" max="16384" width="10.83203125" style="5"/>
+    <col min="16" max="16384" width="10.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>38</v>
       </c>
@@ -968,7 +976,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1">
+    <row r="2" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="11"/>
@@ -991,7 +999,7 @@
       <c r="N2" s="11"/>
       <c r="O2" s="11"/>
     </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1">
+    <row r="3" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="11"/>
@@ -1014,7 +1022,7 @@
       <c r="N3" s="11"/>
       <c r="O3" s="11"/>
     </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" ht="53" customHeight="1">
+    <row r="4" spans="1:15" s="1" customFormat="1" ht="53.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="11"/>
@@ -1037,7 +1045,7 @@
       <c r="N4" s="11"/>
       <c r="O4" s="11"/>
     </row>
-    <row r="5" spans="1:15" s="1" customFormat="1" ht="51.5" customHeight="1">
+    <row r="5" spans="1:15" s="1" customFormat="1" ht="51.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1060,7 +1068,7 @@
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
     </row>
-    <row r="6" spans="1:15" s="1" customFormat="1" ht="20" customHeight="1">
+    <row r="6" spans="1:15" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="5" t="s">
         <v>44</v>
@@ -1079,7 +1087,7 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
     </row>
-    <row r="7" spans="1:15" s="1" customFormat="1" ht="30" customHeight="1">
+    <row r="7" spans="1:15" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>39</v>
       </c>
@@ -1097,7 +1105,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" spans="1:15" s="1" customFormat="1" ht="30" customHeight="1">
+    <row r="8" spans="1:15" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="1" t="s">
@@ -1121,7 +1129,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" spans="1:15" s="1" customFormat="1" ht="30" customHeight="1">
+    <row r="9" spans="1:15" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5" t="s">
         <v>33</v>
@@ -1140,7 +1148,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" spans="1:15" s="1" customFormat="1">
+    <row r="10" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -1167,7 +1175,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" spans="1:15" s="1" customFormat="1">
+    <row r="11" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1192,7 +1200,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" spans="1:15" s="1" customFormat="1">
+    <row r="12" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1217,7 +1225,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" spans="1:15" s="1" customFormat="1">
+    <row r="13" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5" t="s">
         <v>34</v>
@@ -1236,7 +1244,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="1:15" s="1" customFormat="1" ht="30">
+    <row r="14" spans="1:15" s="1" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1267,7 +1275,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" spans="1:15" s="1" customFormat="1" ht="29" customHeight="1">
+    <row r="15" spans="1:15" s="1" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="5" t="s">
         <v>45</v>
@@ -1288,7 +1296,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" spans="1:15" s="1" customFormat="1" ht="39" customHeight="1">
+    <row r="16" spans="1:15" s="1" customFormat="1" ht="38.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1317,7 +1325,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="1" customFormat="1" ht="24" customHeight="1">
+    <row r="17" spans="1:15" s="1" customFormat="1" ht="24.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="s">
         <v>46</v>
@@ -1338,7 +1346,7 @@
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
     </row>
-    <row r="18" spans="1:15" s="1" customFormat="1" ht="29" customHeight="1">
+    <row r="18" spans="1:15" s="1" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="5" t="s">
         <v>44</v>
@@ -1357,7 +1365,7 @@
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
     </row>
-    <row r="19" spans="1:15" s="1" customFormat="1">
+    <row r="19" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="5" t="s">
         <v>47</v>
@@ -1376,7 +1384,7 @@
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
     </row>
-    <row r="20" spans="1:15" s="1" customFormat="1">
+    <row r="20" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="5" t="s">
         <v>48</v>
@@ -1395,7 +1403,7 @@
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
     </row>
-    <row r="21" spans="1:15" s="1" customFormat="1">
+    <row r="21" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5" t="s">
         <v>49</v>
@@ -1414,7 +1422,7 @@
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
     </row>
-    <row r="22" spans="1:15" s="8" customFormat="1">
+    <row r="22" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D22" s="5"/>
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
@@ -1444,17 +1452,17 @@
       <selection activeCell="A7" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="5"/>
-    <col min="3" max="3" width="19.5" style="5" customWidth="1"/>
+    <col min="1" max="1" width="20.77734375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" style="5"/>
+    <col min="3" max="3" width="19.44140625" style="5" customWidth="1"/>
     <col min="4" max="4" width="16" style="5" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="5"/>
+    <col min="5" max="5" width="11.109375" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="10.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>6</v>
       </c>
@@ -1474,7 +1482,7 @@
       <c r="K1" s="13"/>
       <c r="L1" s="13"/>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1">
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>3</v>
       </c>
@@ -1492,7 +1500,7 @@
       <c r="K2" s="13"/>
       <c r="L2" s="13"/>
     </row>
-    <row r="3" spans="1:12" s="1" customFormat="1">
+    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>9</v>
       </c>
@@ -1510,7 +1518,7 @@
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
     </row>
-    <row r="4" spans="1:12" s="1" customFormat="1">
+    <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>10</v>
       </c>
@@ -1528,7 +1536,7 @@
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:12" s="1" customFormat="1">
+    <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>11</v>
       </c>
@@ -1546,7 +1554,7 @@
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" s="1" customFormat="1">
+    <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>66</v>
       </c>
@@ -1564,7 +1572,7 @@
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="1:12" s="1" customFormat="1">
+    <row r="7" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>96</v>
       </c>
@@ -1582,7 +1590,7 @@
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
     </row>
-    <row r="8" spans="1:12" s="1" customFormat="1">
+    <row r="8" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -1596,7 +1604,7 @@
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:12" s="1" customFormat="1">
+    <row r="9" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -1610,7 +1618,7 @@
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12" s="1" customFormat="1">
+    <row r="10" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13"/>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
@@ -1624,7 +1632,7 @@
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
     </row>
-    <row r="11" spans="1:12" s="1" customFormat="1">
+    <row r="11" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
@@ -1638,7 +1646,7 @@
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
     </row>
-    <row r="12" spans="1:12" s="1" customFormat="1">
+    <row r="12" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
@@ -1652,7 +1660,7 @@
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
     </row>
-    <row r="13" spans="1:12" s="1" customFormat="1">
+    <row r="13" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -1666,7 +1674,7 @@
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
     </row>
-    <row r="14" spans="1:12" s="1" customFormat="1">
+    <row r="14" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -1680,7 +1688,7 @@
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
     </row>
-    <row r="15" spans="1:12" s="1" customFormat="1">
+    <row r="15" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13"/>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
@@ -1694,7 +1702,7 @@
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
     </row>
-    <row r="16" spans="1:12" s="8" customFormat="1"/>
+    <row r="16" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1714,13 +1722,13 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.5" customHeight="1">
+    <row r="1" spans="1:2" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -1728,7 +1736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.5" customHeight="1">
+    <row r="2" spans="1:2" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -1736,7 +1744,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -1744,7 +1752,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1752,7 +1760,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1760,7 +1768,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -1768,7 +1776,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -1794,13 +1802,13 @@
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="16.77734375" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="17" customFormat="1" ht="24.5" customHeight="1">
+    <row r="1" spans="1:3" s="17" customFormat="1" ht="24.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1811,7 +1819,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1819,7 +1827,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1830,7 +1838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>29</v>
       </c>
@@ -1841,7 +1849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1870,13 +1878,13 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" customWidth="1"/>
-    <col min="2" max="2" width="170.83203125" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
+    <col min="2" max="2" width="170.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>36</v>
       </c>
@@ -1884,7 +1892,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1910,15 +1918,15 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
     <col min="2" max="4" width="18.6640625" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
     <col min="6" max="9" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.5" customHeight="1">
+    <row r="1" spans="1:8" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>52</v>
       </c>
@@ -1944,7 +1952,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18" customHeight="1">
+    <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>60</v>
       </c>
@@ -1986,7 +1994,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2001,18 +2009,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
     <col min="3" max="3" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>81</v>
       </c>
@@ -2023,7 +2031,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>80</v>
       </c>
@@ -2035,7 +2043,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>80</v>
       </c>
@@ -2047,7 +2055,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>80</v>
       </c>
@@ -2059,7 +2067,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>80</v>
       </c>
@@ -2071,169 +2079,169 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>

</xml_diff>

<commit_message>
Another partial check-in. All table html files have been updated.
</commit_message>
<xml_diff>
--- a/app/config/tables/agriculture/forms/agriculture/agriculture.xlsx
+++ b/app/config/tables/agriculture/forms/agriculture/agriculture.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3535" yWindow="1479" windowWidth="35044" windowHeight="20422" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3535" yWindow="1479" windowWidth="35044" windowHeight="20422" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="107">
   <si>
     <t>name</t>
   </si>
@@ -199,9 +199,6 @@
     <t>selectionArgs</t>
   </si>
   <si>
-    <t>auxillaryHash</t>
-  </si>
-  <si>
     <t>linked_table</t>
   </si>
   <si>
@@ -214,9 +211,6 @@
     <t>values_list</t>
   </si>
   <si>
-    <t>''</t>
-  </si>
-  <si>
     <t>fieldName</t>
   </si>
   <si>
@@ -350,6 +344,15 @@
   </si>
   <si>
     <t>display.constraint_message.text</t>
+  </si>
+  <si>
+    <t>newRowInitialElementKeyToValueMap</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>openRowInitialElementKeyToValueMap</t>
   </si>
 </sst>
 </file>
@@ -972,25 +975,25 @@
         <v>0</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G1" s="16" t="s">
         <v>26</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I1" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="K1" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>102</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>104</v>
       </c>
       <c r="M1" s="6" t="s">
         <v>2</v>
@@ -999,7 +1002,7 @@
         <v>29</v>
       </c>
       <c r="O1" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1014,7 +1017,7 @@
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H2" s="16"/>
       <c r="I2" s="16"/>
@@ -1037,7 +1040,7 @@
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
@@ -1060,7 +1063,7 @@
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H4" s="16"/>
       <c r="I4" s="16"/>
@@ -1135,17 +1138,17 @@
       <c r="A8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
@@ -1179,19 +1182,19 @@
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1212,7 +1215,7 @@
         <v>27</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5" t="b">
@@ -1237,7 +1240,7 @@
         <v>28</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5" t="b">
@@ -1287,13 +1290,13 @@
         <v>22</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K14" s="5" t="s">
         <v>23</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M14" s="5" t="b">
         <v>1</v>
@@ -1337,10 +1340,10 @@
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L16" s="5"/>
       <c r="M16" s="6"/>
@@ -1348,7 +1351,7 @@
         <v>48</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:15" s="1" customFormat="1" ht="24.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -1474,7 +1477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1496,7 +1499,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
@@ -1582,10 +1585,10 @@
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
@@ -1600,7 +1603,7 @@
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B7" s="19" t="b">
         <v>1</v>
@@ -1842,7 +1845,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1858,7 +1861,7 @@
         <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
@@ -1923,7 +1926,7 @@
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1938,10 +1941,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1949,10 +1952,12 @@
     <col min="1" max="1" width="15.109375" customWidth="1"/>
     <col min="2" max="4" width="18.6640625" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="9" width="18.6640625" customWidth="1"/>
+    <col min="6" max="7" width="18.6640625" customWidth="1"/>
+    <col min="8" max="8" width="35.88671875" customWidth="1"/>
+    <col min="9" max="9" width="35.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>49</v>
       </c>
@@ -1972,18 +1977,21 @@
         <v>54</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H1" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -1992,16 +2000,19 @@
         <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>60</v>
+        <v>105</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2048,10 +2059,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -2059,49 +2070,49 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2299,13 +2310,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" t="s">
         <v>93</v>
-      </c>
-      <c r="B1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C1" t="s">
-        <v>95</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -2316,19 +2327,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" t="s">
         <v>98</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>97</v>
-      </c>
-      <c r="C2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E2" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>